<commit_message>
new input with test
</commit_message>
<xml_diff>
--- a/New_input/ANTIBIOTIC ANTIFUNGAL ANTIVIRAL.xlsx
+++ b/New_input/ANTIBIOTIC ANTIFUNGAL ANTIVIRAL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvin Buana\Documents\Alvin\pukulEnam\Consultant Projects_\product_performance_blstm\New_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF9ED8C-C1D2-455F-8A5B-22CA28C94252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7913151-AE68-4717-8D3F-8F6023490FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{276185C5-1ECF-4C6D-8A86-C1AD4F169BB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{276185C5-1ECF-4C6D-8A86-C1AD4F169BB5}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>
@@ -174,12 +174,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E0335A-0128-4D17-A0C7-4F5312672E70}">
   <dimension ref="A1:BD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BI15" sqref="BI15"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AZ25" sqref="AZ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,71 +522,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-      <c r="BC1" s="7"/>
-      <c r="BD1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -743,7 +749,7 @@
       <c r="BC2" s="1">
         <v>54</v>
       </c>
-      <c r="BD2" s="6"/>
+      <c r="BD2" s="8"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -3647,10 +3653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390B4544-74FC-40FB-BB5F-73D443B04A04}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3659,199 +3665,241 @@
     <col min="8" max="8" width="22.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="5" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
       <c r="B2" s="1">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1">
         <v>55</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E2" s="1">
         <v>56</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>57</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>58</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>59</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <v>60</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="E3" s="3">
         <v>19</v>
       </c>
-      <c r="D3" s="3">
+      <c r="F3" s="3">
         <v>57</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
+      <c r="H3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="3">
-        <v>20</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="3">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <v>16</v>
       </c>
-      <c r="E4" s="3">
+      <c r="G4" s="3">
         <v>9</v>
       </c>
-      <c r="F4" s="3">
+      <c r="H4" s="3">
         <v>8</v>
       </c>
-      <c r="G4" s="3">
+      <c r="I4" s="3">
         <v>4</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="3">
+      <c r="E5" s="3">
         <v>13</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="H5" s="3">
         <v>4</v>
       </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
+        <v>511</v>
+      </c>
+      <c r="C6" s="3">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3">
         <v>1079</v>
       </c>
-      <c r="C6" s="3">
+      <c r="E6" s="3">
         <v>302</v>
       </c>
-      <c r="D6" s="3">
+      <c r="F6" s="3">
         <v>1596</v>
       </c>
-      <c r="E6" s="3">
+      <c r="G6" s="3">
         <v>9</v>
       </c>
-      <c r="F6" s="3">
+      <c r="H6" s="3">
         <v>114</v>
       </c>
-      <c r="G6" s="3">
+      <c r="I6" s="3">
         <v>28</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3">
         <v>45</v>
       </c>
-      <c r="C7" s="3">
+      <c r="E7" s="3">
         <v>87</v>
       </c>
-      <c r="D7" s="3">
+      <c r="F7" s="3">
         <v>16</v>
       </c>
-      <c r="E7" s="3">
+      <c r="G7" s="3">
         <v>28</v>
       </c>
-      <c r="F7" s="3">
+      <c r="H7" s="3">
         <v>22</v>
       </c>
-      <c r="G7" s="3">
+      <c r="I7" s="3">
         <v>15</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3">
         <v>62</v>
       </c>
-      <c r="C8" s="3">
+      <c r="E8" s="3">
         <v>112</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <v>48</v>
       </c>
-      <c r="E8" s="3">
+      <c r="G8" s="3">
         <v>41</v>
       </c>
-      <c r="F8" s="3">
+      <c r="H8" s="3">
         <v>34</v>
       </c>
-      <c r="G8" s="3">
+      <c r="I8" s="3">
         <v>54</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3859,51 +3907,63 @@
         <v>3</v>
       </c>
       <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
         <v>10</v>
       </c>
-      <c r="D9" s="3">
+      <c r="F9" s="3">
         <v>22</v>
       </c>
-      <c r="E9" s="3">
+      <c r="G9" s="3">
         <v>5</v>
       </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3">
         <v>26</v>
       </c>
-      <c r="C10" s="3">
+      <c r="E10" s="3">
         <v>50</v>
-      </c>
-      <c r="D10" s="3">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3">
-        <v>43</v>
       </c>
       <c r="F10" s="3">
         <v>40</v>
       </c>
       <c r="G10" s="3">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3">
         <v>46</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -3911,25 +3971,31 @@
         <v>1</v>
       </c>
       <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
         <v>4</v>
       </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
       <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
         <v>11</v>
       </c>
-      <c r="G11" s="3">
+      <c r="I11" s="3">
         <v>-11</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -3951,167 +4017,209 @@
       <c r="G12" s="3">
         <v>0</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3">
+        <v>61</v>
+      </c>
+      <c r="C13" s="3">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3">
         <v>48</v>
       </c>
-      <c r="C13" s="3">
+      <c r="E13" s="3">
         <v>76</v>
       </c>
-      <c r="D13" s="3">
+      <c r="F13" s="3">
         <v>82</v>
       </c>
-      <c r="E13" s="3">
+      <c r="G13" s="3">
         <v>24</v>
       </c>
-      <c r="F13" s="3">
+      <c r="H13" s="3">
         <v>30</v>
       </c>
-      <c r="G13" s="3">
+      <c r="I13" s="3">
         <v>-1</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="3">
+      <c r="E14" s="3">
         <v>9</v>
       </c>
-      <c r="D14" s="3">
+      <c r="F14" s="3">
         <v>6</v>
       </c>
-      <c r="E14" s="3">
+      <c r="G14" s="3">
         <v>8</v>
       </c>
-      <c r="F14" s="3">
+      <c r="H14" s="3">
         <v>7</v>
       </c>
-      <c r="G14" s="3">
+      <c r="I14" s="3">
         <v>4</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
         <v>18</v>
       </c>
-      <c r="D15" s="3">
+      <c r="F15" s="3">
         <v>29</v>
       </c>
-      <c r="E15" s="3">
+      <c r="G15" s="3">
         <v>6</v>
       </c>
-      <c r="F15" s="3">
+      <c r="H15" s="3">
         <v>18</v>
       </c>
-      <c r="G15" s="3">
+      <c r="I15" s="3">
         <v>10</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="3">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
         <v>27</v>
       </c>
-      <c r="C16" s="3">
+      <c r="E16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="3">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
+      <c r="G16" s="3">
         <v>42</v>
       </c>
-      <c r="F16" s="3">
+      <c r="H16" s="3">
         <v>6</v>
       </c>
-      <c r="G16" s="3">
+      <c r="I16" s="3">
         <v>40</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="3">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3">
         <v>38</v>
       </c>
-      <c r="C17" s="3">
+      <c r="E17" s="3">
         <v>35</v>
       </c>
-      <c r="D17" s="3">
+      <c r="F17" s="3">
         <v>10</v>
       </c>
-      <c r="E17" s="3">
+      <c r="G17" s="3">
         <v>28</v>
       </c>
-      <c r="F17" s="3">
+      <c r="H17" s="3">
         <v>25</v>
       </c>
-      <c r="G17" s="3">
+      <c r="I17" s="3">
         <v>49</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="3">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
         <v>39</v>
       </c>
-      <c r="C18" s="3">
+      <c r="E18" s="3">
         <v>79</v>
       </c>
-      <c r="D18" s="3">
+      <c r="F18" s="3">
         <v>91</v>
       </c>
-      <c r="E18" s="3">
+      <c r="G18" s="3">
         <v>119</v>
       </c>
-      <c r="F18" s="3">
+      <c r="H18" s="3">
         <v>112</v>
       </c>
-      <c r="G18" s="3">
+      <c r="I18" s="3">
         <v>25</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -4133,15 +4241,20 @@
       <c r="G19" s="3">
         <v>0</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>